<commit_message>
back connection loco also works + tp routing
</commit_message>
<xml_diff>
--- a/ExcelOutput/Positions.xlsx
+++ b/ExcelOutput/Positions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Loco 0 pos</t>
   </si>
@@ -22,7 +22,10 @@
     <t>TP 0 pos</t>
   </si>
   <si>
-    <t>Loco 0 connected to TP</t>
+    <t>Loco 0 front connection to TP</t>
+  </si>
+  <si>
+    <t>Loco 0 back connection to TP</t>
   </si>
   <si>
     <t>TP 0 moveable flag</t>
@@ -383,13 +386,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,127 +405,151 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="D2">
         <v>-1</v>
       </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2">
+        <v>-1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>-1</v>
       </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3">
+        <v>-1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>-1</v>
       </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>-1</v>
       </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5">
+        <v>-1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>-1</v>
       </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>-1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>-1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -530,131 +557,155 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>-1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>-1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>-1</v>
       </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="E11">
+        <v>-1</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>-1</v>
       </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="E12">
+        <v>-1</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>-1</v>
       </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="E13">
+        <v>-1</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D14">
         <v>-1</v>
       </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="E14">
+        <v>-1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15">
         <v>-1</v>
       </c>
-      <c r="E15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="E15">
+        <v>-1</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D16">
         <v>-1</v>
       </c>
-      <c r="E16" t="b">
+      <c r="E16">
+        <v>-1</v>
+      </c>
+      <c r="F16" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
import torpedodata + generation of first 5 tp snapshot
</commit_message>
<xml_diff>
--- a/ExcelOutput/Positions.xlsx
+++ b/ExcelOutput/Positions.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,19 +414,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="D2">
         <v>-1</v>
       </c>
       <c r="E2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -434,19 +434,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D3">
         <v>-1</v>
       </c>
       <c r="E3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -454,16 +454,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>-1</v>
       </c>
       <c r="E4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -474,10 +474,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="D5">
         <v>-1</v>
@@ -494,16 +494,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="D6">
         <v>-1</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -514,19 +514,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="D7">
         <v>-1</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -534,19 +534,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D8">
         <v>-1</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -554,19 +554,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D9">
         <v>-1</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -574,16 +574,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D10">
         <v>-1</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -594,10 +594,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D11">
         <v>-1</v>
@@ -614,10 +614,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D12">
         <v>-1</v>
@@ -634,10 +634,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D13">
         <v>-1</v>
@@ -654,10 +654,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D14">
         <v>-1</v>
@@ -674,19 +674,19 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D15">
         <v>-1</v>
       </c>
       <c r="E15">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -694,18 +694,1718 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="D16">
         <v>-1</v>
       </c>
       <c r="E16">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>45</v>
+      </c>
+      <c r="C17">
+        <v>44</v>
+      </c>
+      <c r="D17">
+        <v>-1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>98</v>
+      </c>
+      <c r="C18">
+        <v>45</v>
+      </c>
+      <c r="D18">
+        <v>-1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>45</v>
+      </c>
+      <c r="C19">
+        <v>44</v>
+      </c>
+      <c r="D19">
+        <v>-1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>98</v>
+      </c>
+      <c r="C20">
+        <v>45</v>
+      </c>
+      <c r="D20">
+        <v>-1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>45</v>
+      </c>
+      <c r="C21">
+        <v>44</v>
+      </c>
+      <c r="D21">
+        <v>-1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>98</v>
+      </c>
+      <c r="C22">
+        <v>45</v>
+      </c>
+      <c r="D22">
+        <v>-1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>45</v>
+      </c>
+      <c r="C23">
+        <v>44</v>
+      </c>
+      <c r="D23">
+        <v>-1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>98</v>
+      </c>
+      <c r="C24">
+        <v>45</v>
+      </c>
+      <c r="D24">
+        <v>-1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>45</v>
+      </c>
+      <c r="C25">
+        <v>44</v>
+      </c>
+      <c r="D25">
+        <v>-1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>98</v>
+      </c>
+      <c r="C26">
+        <v>45</v>
+      </c>
+      <c r="D26">
+        <v>-1</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>45</v>
+      </c>
+      <c r="C27">
+        <v>44</v>
+      </c>
+      <c r="D27">
+        <v>-1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>98</v>
+      </c>
+      <c r="C28">
+        <v>45</v>
+      </c>
+      <c r="D28">
+        <v>-1</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>45</v>
+      </c>
+      <c r="C29">
+        <v>44</v>
+      </c>
+      <c r="D29">
+        <v>-1</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>98</v>
+      </c>
+      <c r="C30">
+        <v>45</v>
+      </c>
+      <c r="D30">
+        <v>-1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>45</v>
+      </c>
+      <c r="C31">
+        <v>44</v>
+      </c>
+      <c r="D31">
+        <v>-1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>98</v>
+      </c>
+      <c r="C32">
+        <v>45</v>
+      </c>
+      <c r="D32">
+        <v>-1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>45</v>
+      </c>
+      <c r="C33">
+        <v>44</v>
+      </c>
+      <c r="D33">
+        <v>-1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>98</v>
+      </c>
+      <c r="C34">
+        <v>45</v>
+      </c>
+      <c r="D34">
+        <v>-1</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>45</v>
+      </c>
+      <c r="C35">
+        <v>44</v>
+      </c>
+      <c r="D35">
+        <v>-1</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>98</v>
+      </c>
+      <c r="C36">
+        <v>45</v>
+      </c>
+      <c r="D36">
+        <v>-1</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>45</v>
+      </c>
+      <c r="C37">
+        <v>44</v>
+      </c>
+      <c r="D37">
+        <v>-1</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>98</v>
+      </c>
+      <c r="C38">
+        <v>45</v>
+      </c>
+      <c r="D38">
+        <v>-1</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>45</v>
+      </c>
+      <c r="C39">
+        <v>44</v>
+      </c>
+      <c r="D39">
+        <v>-1</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>98</v>
+      </c>
+      <c r="C40">
+        <v>45</v>
+      </c>
+      <c r="D40">
+        <v>-1</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>45</v>
+      </c>
+      <c r="C41">
+        <v>44</v>
+      </c>
+      <c r="D41">
+        <v>-1</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>98</v>
+      </c>
+      <c r="C42">
+        <v>45</v>
+      </c>
+      <c r="D42">
+        <v>-1</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>45</v>
+      </c>
+      <c r="C43">
+        <v>44</v>
+      </c>
+      <c r="D43">
+        <v>-1</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>98</v>
+      </c>
+      <c r="C44">
+        <v>45</v>
+      </c>
+      <c r="D44">
+        <v>-1</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>45</v>
+      </c>
+      <c r="C45">
+        <v>44</v>
+      </c>
+      <c r="D45">
+        <v>-1</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>98</v>
+      </c>
+      <c r="C46">
+        <v>45</v>
+      </c>
+      <c r="D46">
+        <v>-1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>45</v>
+      </c>
+      <c r="C47">
+        <v>44</v>
+      </c>
+      <c r="D47">
+        <v>-1</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>98</v>
+      </c>
+      <c r="C48">
+        <v>45</v>
+      </c>
+      <c r="D48">
+        <v>-1</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>45</v>
+      </c>
+      <c r="C49">
+        <v>44</v>
+      </c>
+      <c r="D49">
+        <v>-1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>98</v>
+      </c>
+      <c r="C50">
+        <v>45</v>
+      </c>
+      <c r="D50">
+        <v>-1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>45</v>
+      </c>
+      <c r="C51">
+        <v>44</v>
+      </c>
+      <c r="D51">
+        <v>-1</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>98</v>
+      </c>
+      <c r="C52">
+        <v>45</v>
+      </c>
+      <c r="D52">
+        <v>-1</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>45</v>
+      </c>
+      <c r="C53">
+        <v>44</v>
+      </c>
+      <c r="D53">
+        <v>-1</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>98</v>
+      </c>
+      <c r="C54">
+        <v>45</v>
+      </c>
+      <c r="D54">
+        <v>-1</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>45</v>
+      </c>
+      <c r="C55">
+        <v>44</v>
+      </c>
+      <c r="D55">
+        <v>-1</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>98</v>
+      </c>
+      <c r="C56">
+        <v>45</v>
+      </c>
+      <c r="D56">
+        <v>-1</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>45</v>
+      </c>
+      <c r="C57">
+        <v>44</v>
+      </c>
+      <c r="D57">
+        <v>-1</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>98</v>
+      </c>
+      <c r="C58">
+        <v>45</v>
+      </c>
+      <c r="D58">
+        <v>-1</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>45</v>
+      </c>
+      <c r="C59">
+        <v>44</v>
+      </c>
+      <c r="D59">
+        <v>-1</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>98</v>
+      </c>
+      <c r="C60">
+        <v>45</v>
+      </c>
+      <c r="D60">
+        <v>-1</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>45</v>
+      </c>
+      <c r="C61">
+        <v>44</v>
+      </c>
+      <c r="D61">
+        <v>-1</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>98</v>
+      </c>
+      <c r="C62">
+        <v>45</v>
+      </c>
+      <c r="D62">
+        <v>-1</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>45</v>
+      </c>
+      <c r="C63">
+        <v>44</v>
+      </c>
+      <c r="D63">
+        <v>-1</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>98</v>
+      </c>
+      <c r="C64">
+        <v>45</v>
+      </c>
+      <c r="D64">
+        <v>-1</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>45</v>
+      </c>
+      <c r="C65">
+        <v>44</v>
+      </c>
+      <c r="D65">
+        <v>-1</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>98</v>
+      </c>
+      <c r="C66">
+        <v>45</v>
+      </c>
+      <c r="D66">
+        <v>-1</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>45</v>
+      </c>
+      <c r="C67">
+        <v>44</v>
+      </c>
+      <c r="D67">
+        <v>-1</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>98</v>
+      </c>
+      <c r="C68">
+        <v>45</v>
+      </c>
+      <c r="D68">
+        <v>-1</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>46</v>
+      </c>
+      <c r="C69">
+        <v>98</v>
+      </c>
+      <c r="D69">
+        <v>-1</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>102</v>
+      </c>
+      <c r="C70">
+        <v>46</v>
+      </c>
+      <c r="D70">
+        <v>-1</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>64</v>
+      </c>
+      <c r="C71">
+        <v>102</v>
+      </c>
+      <c r="D71">
+        <v>-1</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>66</v>
+      </c>
+      <c r="C72">
+        <v>64</v>
+      </c>
+      <c r="D72">
+        <v>-1</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>109</v>
+      </c>
+      <c r="C73">
+        <v>66</v>
+      </c>
+      <c r="D73">
+        <v>-1</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>66</v>
+      </c>
+      <c r="C74">
+        <v>110</v>
+      </c>
+      <c r="D74">
+        <v>-1</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>110</v>
+      </c>
+      <c r="C75">
+        <v>111</v>
+      </c>
+      <c r="D75">
+        <v>-1</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>111</v>
+      </c>
+      <c r="C76">
+        <v>112</v>
+      </c>
+      <c r="D76">
+        <v>-1</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>112</v>
+      </c>
+      <c r="C77">
+        <v>113</v>
+      </c>
+      <c r="D77">
+        <v>-1</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>113</v>
+      </c>
+      <c r="C78">
+        <v>72</v>
+      </c>
+      <c r="D78">
+        <v>-1</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>72</v>
+      </c>
+      <c r="C79">
+        <v>114</v>
+      </c>
+      <c r="D79">
+        <v>-1</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>114</v>
+      </c>
+      <c r="C80">
+        <v>69</v>
+      </c>
+      <c r="D80">
+        <v>-1</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>69</v>
+      </c>
+      <c r="C81">
+        <v>70</v>
+      </c>
+      <c r="D81">
+        <v>-1</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>70</v>
+      </c>
+      <c r="C82">
+        <v>115</v>
+      </c>
+      <c r="D82">
+        <v>-1</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>115</v>
+      </c>
+      <c r="C83">
+        <v>116</v>
+      </c>
+      <c r="D83">
+        <v>-1</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>116</v>
+      </c>
+      <c r="C84">
+        <v>117</v>
+      </c>
+      <c r="D84">
+        <v>-1</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>117</v>
+      </c>
+      <c r="C85">
+        <v>118</v>
+      </c>
+      <c r="D85">
+        <v>-1</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>118</v>
+      </c>
+      <c r="C86">
+        <v>119</v>
+      </c>
+      <c r="D86">
+        <v>-1</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>119</v>
+      </c>
+      <c r="C87">
+        <v>120</v>
+      </c>
+      <c r="D87">
+        <v>-1</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>120</v>
+      </c>
+      <c r="C88">
+        <v>121</v>
+      </c>
+      <c r="D88">
+        <v>-1</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>121</v>
+      </c>
+      <c r="C89">
+        <v>71</v>
+      </c>
+      <c r="D89">
+        <v>-1</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>71</v>
+      </c>
+      <c r="C90">
+        <v>132</v>
+      </c>
+      <c r="D90">
+        <v>-1</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>132</v>
+      </c>
+      <c r="C91">
+        <v>36</v>
+      </c>
+      <c r="D91">
+        <v>-1</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>36</v>
+      </c>
+      <c r="C92">
+        <v>41</v>
+      </c>
+      <c r="D92">
+        <v>-1</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>41</v>
+      </c>
+      <c r="C93">
+        <v>40</v>
+      </c>
+      <c r="D93">
+        <v>-1</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>40</v>
+      </c>
+      <c r="C94">
+        <v>35</v>
+      </c>
+      <c r="D94">
+        <v>-1</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>35</v>
+      </c>
+      <c r="C95">
+        <v>37</v>
+      </c>
+      <c r="D95">
+        <v>-1</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>37</v>
+      </c>
+      <c r="C96">
+        <v>32</v>
+      </c>
+      <c r="D96">
+        <v>-1</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>32</v>
+      </c>
+      <c r="C97">
+        <v>154</v>
+      </c>
+      <c r="D97">
+        <v>-1</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>154</v>
+      </c>
+      <c r="C98">
+        <v>155</v>
+      </c>
+      <c r="D98">
+        <v>-1</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>155</v>
+      </c>
+      <c r="C99">
+        <v>27</v>
+      </c>
+      <c r="D99">
+        <v>-1</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>155</v>
+      </c>
+      <c r="C100">
+        <v>27</v>
+      </c>
+      <c r="D100">
+        <v>-1</v>
+      </c>
+      <c r="E100">
+        <v>-1</v>
+      </c>
+      <c r="F100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>155</v>
+      </c>
+      <c r="C101">
+        <v>27</v>
+      </c>
+      <c r="D101">
+        <v>-1</v>
+      </c>
+      <c r="E101">
+        <v>-1</v>
+      </c>
+      <c r="F101" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>